<commit_message>
21 Nov no. 1
</commit_message>
<xml_diff>
--- a/01.MODELO PERSEPOLIS/02.Ejecucion/02.Frente Operacion/Entregables Especialistas/Salud/SIPOC - Saludv7.xlsx
+++ b/01.MODELO PERSEPOLIS/02.Ejecucion/02.Frente Operacion/Entregables Especialistas/Salud/SIPOC - Saludv7.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harry Wong\Dropbox\privada\Persepolis\01.MODELO PERSEPOLIS\02.Ejecucion\02.Frente Operacion\Entregables Especialistas\Salud\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Salud" sheetId="1" r:id="rId1"/>
     <sheet name="indicadores" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1443,7 +1448,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1483,6 +1488,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1551,7 +1562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1626,9 +1637,45 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1647,61 +1694,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1769,7 +1796,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1804,7 +1831,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2015,11 +2042,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="34" zoomScaleNormal="34" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="S82" sqref="S82"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.3"/>
@@ -2041,53 +2068,53 @@
     <col min="29" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+    <row r="2" spans="2:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-    </row>
-    <row r="3" spans="2:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+    </row>
+    <row r="3" spans="2:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="42" t="s">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-    </row>
-    <row r="4" spans="2:19" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
+      <c r="S3" s="34"/>
+    </row>
+    <row r="4" spans="2:21" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
@@ -2143,112 +2170,112 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+    <row r="5" spans="2:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="38" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="31" t="s">
         <v>138</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="44"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="43" t="s">
+      <c r="F5" s="37"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="L5" s="43" t="s">
+      <c r="L5" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="35" t="s">
+      <c r="M5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="43" t="s">
+      <c r="N5" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="26" t="s">
+      <c r="P5" s="31" t="s">
         <v>14</v>
       </c>
       <c r="Q5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="R5" s="40" t="s">
+      <c r="R5" s="33" t="s">
         <v>36</v>
       </c>
       <c r="S5" s="21"/>
     </row>
-    <row r="6" spans="2:19" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="45"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="43"/>
-      <c r="O6" s="44"/>
-      <c r="P6" s="26"/>
+    <row r="6" spans="2:21" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="38"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="31"/>
       <c r="Q6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="R6" s="40"/>
+      <c r="R6" s="33"/>
       <c r="S6" s="21"/>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="45"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="44"/>
-      <c r="P7" s="26"/>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B7" s="38"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="26"/>
+      <c r="L7" s="36"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="36"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="31"/>
       <c r="Q7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R7" s="40"/>
+      <c r="R7" s="33"/>
       <c r="S7" s="21"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B8" s="45"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="40"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="43"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="43"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="26"/>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
+      <c r="B8" s="38"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="36"/>
+      <c r="K8" s="26"/>
+      <c r="L8" s="36"/>
+      <c r="M8" s="26"/>
+      <c r="N8" s="36"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="31"/>
       <c r="Q8" s="9" t="s">
         <v>20</v>
       </c>
@@ -2257,17 +2284,17 @@
       </c>
       <c r="S8" s="21"/>
     </row>
-    <row r="9" spans="2:19" ht="85.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="45"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="35"/>
+    <row r="9" spans="2:21" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="38"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="36"/>
+      <c r="K9" s="26"/>
       <c r="L9" s="18" t="s">
         <v>11</v>
       </c>
@@ -2291,17 +2318,17 @@
       </c>
       <c r="S9" s="21"/>
     </row>
-    <row r="10" spans="2:19" ht="57" x14ac:dyDescent="0.3">
-      <c r="B10" s="45"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="35"/>
+    <row r="10" spans="2:21" ht="57" x14ac:dyDescent="0.3">
+      <c r="B10" s="38"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="37"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="37"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="26"/>
       <c r="L10" s="18" t="s">
         <v>12</v>
       </c>
@@ -2325,17 +2352,17 @@
       </c>
       <c r="S10" s="21"/>
     </row>
-    <row r="11" spans="2:19" ht="57" x14ac:dyDescent="0.3">
-      <c r="B11" s="45"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="44"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="35"/>
+    <row r="11" spans="2:21" ht="57" x14ac:dyDescent="0.3">
+      <c r="B11" s="38"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="26"/>
       <c r="L11" s="18" t="s">
         <v>9</v>
       </c>
@@ -2359,17 +2386,17 @@
       </c>
       <c r="S11" s="21"/>
     </row>
-    <row r="12" spans="2:19" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="45"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="35"/>
+    <row r="12" spans="2:21" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="38"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="26"/>
       <c r="L12" s="7" t="s">
         <v>21</v>
       </c>
@@ -2393,599 +2420,615 @@
       </c>
       <c r="S12" s="21"/>
     </row>
-    <row r="13" spans="2:19" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="36" t="s">
+    <row r="13" spans="2:21" s="48" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="38"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="47" t="s">
         <v>126</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="47" t="s">
         <v>140</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="K13" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="L13" s="8" t="s">
+      <c r="L13" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="N13" s="8" t="s">
+      <c r="N13" s="47" t="s">
         <v>143</v>
       </c>
-      <c r="O13" s="16"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="16" t="s">
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="14" spans="2:19" ht="165" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="45"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="36" t="s">
+      <c r="U13" s="49"/>
+    </row>
+    <row r="14" spans="2:21" s="48" customFormat="1" ht="165" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="38"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="45" t="s">
         <v>287</v>
       </c>
-      <c r="J14" s="35" t="s">
+      <c r="J14" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="35" t="s">
+      <c r="K14" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="L14" s="35" t="s">
+      <c r="L14" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" s="47" t="s">
         <v>284</v>
       </c>
-      <c r="N14" s="8" t="s">
+      <c r="N14" s="47" t="s">
         <v>288</v>
       </c>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="P14" s="11" t="s">
+      <c r="P14" s="47" t="s">
         <v>289</v>
       </c>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11" t="s">
+      <c r="Q14" s="47"/>
+      <c r="R14" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="S14" s="16" t="s">
+      <c r="S14" s="47" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="15" spans="2:19" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="45"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="8" t="s">
+      <c r="U14" s="49"/>
+    </row>
+    <row r="15" spans="2:21" s="48" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="38"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
+      <c r="K15" s="45"/>
+      <c r="L15" s="45"/>
+      <c r="M15" s="47" t="s">
         <v>106</v>
       </c>
-      <c r="N15" s="8" t="s">
+      <c r="N15" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="O15" s="16" t="s">
+      <c r="O15" s="47" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="11" t="s">
+      <c r="P15" s="47" t="s">
         <v>286</v>
       </c>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11" t="s">
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="S15" s="16" t="s">
+      <c r="S15" s="47" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="16" spans="2:19" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="45"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="36" t="s">
+      <c r="U15" s="49"/>
+    </row>
+    <row r="16" spans="2:21" s="48" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="38"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45" t="s">
         <v>290</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="45" t="s">
         <v>291</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="H16" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="47" t="s">
         <v>292</v>
       </c>
-      <c r="J16" s="8" t="s">
+      <c r="J16" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="K16" s="8" t="s">
+      <c r="K16" s="47" t="s">
         <v>152</v>
       </c>
-      <c r="L16" s="8" t="s">
+      <c r="L16" s="47" t="s">
         <v>58</v>
       </c>
-      <c r="M16" s="8" t="s">
+      <c r="M16" s="47" t="s">
         <v>153</v>
       </c>
-      <c r="N16" s="8" t="s">
+      <c r="N16" s="47" t="s">
         <v>154</v>
       </c>
-      <c r="O16" s="16"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="16" t="s">
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="47" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="17" spans="2:20" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="45"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="16" t="s">
+      <c r="U16" s="49"/>
+    </row>
+    <row r="17" spans="2:21" s="48" customFormat="1" ht="71.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="38"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="47" t="s">
         <v>293</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="47" t="s">
         <v>158</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="K17" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="L17" s="8" t="s">
+      <c r="L17" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="M17" s="8" t="s">
+      <c r="M17" s="47" t="s">
         <v>160</v>
       </c>
-      <c r="N17" s="8" t="s">
+      <c r="N17" s="47" t="s">
         <v>161</v>
       </c>
-      <c r="O17" s="16"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="16" t="s">
+      <c r="O17" s="47"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="47"/>
+      <c r="S17" s="47" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="18" spans="2:20" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="45"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="16" t="s">
+      <c r="U17" s="49"/>
+    </row>
+    <row r="18" spans="2:21" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B18" s="38"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I18" s="47" t="s">
         <v>295</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="47" t="s">
         <v>162</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="47" t="s">
         <v>165</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="8" t="s">
+      <c r="M18" s="47" t="s">
         <v>163</v>
       </c>
-      <c r="N18" s="8" t="s">
+      <c r="N18" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O18" s="16"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="16" t="s">
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="47" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="19" spans="2:20" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="45"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="16" t="s">
+      <c r="U18" s="49"/>
+    </row>
+    <row r="19" spans="2:21" s="48" customFormat="1" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="38"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="I19" s="11" t="s">
+      <c r="I19" s="47" t="s">
         <v>296</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="47" t="s">
         <v>166</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="K19" s="47" t="s">
         <v>167</v>
       </c>
-      <c r="L19" s="8" t="s">
+      <c r="L19" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="M19" s="8" t="s">
+      <c r="M19" s="47" t="s">
         <v>168</v>
       </c>
-      <c r="N19" s="8" t="s">
+      <c r="N19" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O19" s="16"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="16" t="s">
+      <c r="O19" s="47"/>
+      <c r="P19" s="47"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="47"/>
+      <c r="S19" s="47" t="s">
         <v>169</v>
       </c>
-      <c r="T19" s="3"/>
-    </row>
-    <row r="20" spans="2:20" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="16" t="s">
+      <c r="T19" s="49"/>
+      <c r="U19" s="49"/>
+    </row>
+    <row r="20" spans="2:21" s="48" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="38"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="47" t="s">
         <v>297</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="L20" s="8" t="s">
+      <c r="L20" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="M20" s="8" t="s">
+      <c r="M20" s="47" t="s">
         <v>171</v>
       </c>
-      <c r="N20" s="8" t="s">
+      <c r="N20" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O20" s="16"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="16" t="s">
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47" t="s">
         <v>172</v>
       </c>
-      <c r="T20" s="3"/>
-    </row>
-    <row r="21" spans="2:20" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="45"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="36" t="s">
+      <c r="T20" s="49"/>
+      <c r="U20" s="49"/>
+    </row>
+    <row r="21" spans="2:21" s="48" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="38"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="26" t="s">
+      <c r="I21" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="47" t="s">
         <v>174</v>
       </c>
-      <c r="L21" s="35" t="s">
+      <c r="L21" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="M21" s="8" t="s">
+      <c r="M21" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="N21" s="8" t="s">
+      <c r="N21" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O21" s="16"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="16" t="s">
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="2:20" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="45"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35" t="s">
+      <c r="U21" s="49"/>
+    </row>
+    <row r="22" spans="2:21" s="48" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="38"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35" t="s">
+      <c r="L22" s="45"/>
+      <c r="M22" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="N22" s="35" t="s">
+      <c r="N22" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="O22" s="16"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="16" t="s">
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="23" spans="2:20" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="45"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="16" t="s">
+      <c r="U22" s="49"/>
+    </row>
+    <row r="23" spans="2:21" s="48" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="38"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
+      <c r="K23" s="45"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="45"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="47"/>
+      <c r="P23" s="47"/>
+      <c r="Q23" s="47"/>
+      <c r="R23" s="47"/>
+      <c r="S23" s="47" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="24" spans="2:20" ht="71.25" x14ac:dyDescent="0.3">
-      <c r="B24" s="45"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="16" t="s">
+      <c r="U23" s="49"/>
+    </row>
+    <row r="24" spans="2:21" s="48" customFormat="1" ht="71.25" x14ac:dyDescent="0.3">
+      <c r="B24" s="38"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="N24" s="8" t="s">
+      <c r="N24" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="O24" s="16"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="16" t="s">
+      <c r="O24" s="47"/>
+      <c r="P24" s="47"/>
+      <c r="Q24" s="47"/>
+      <c r="R24" s="47"/>
+      <c r="S24" s="47" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="25" spans="2:20" ht="85.5" x14ac:dyDescent="0.3">
-      <c r="B25" s="45"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="16" t="s">
+      <c r="U24" s="49"/>
+    </row>
+    <row r="25" spans="2:21" s="48" customFormat="1" ht="85.5" x14ac:dyDescent="0.3">
+      <c r="B25" s="38"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="45"/>
+      <c r="H25" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="47" t="s">
         <v>300</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="47" t="s">
         <v>155</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="L25" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="N25" s="8" t="s">
+      <c r="N25" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="O25" s="16"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="16" t="s">
+      <c r="O25" s="47"/>
+      <c r="P25" s="47"/>
+      <c r="Q25" s="47"/>
+      <c r="R25" s="47"/>
+      <c r="S25" s="47" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="26" spans="2:20" ht="42.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="45"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="16" t="s">
+      <c r="U25" s="49"/>
+    </row>
+    <row r="26" spans="2:21" s="48" customFormat="1" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="38"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="47" t="s">
         <v>302</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="K26" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="L26" s="8" t="s">
+      <c r="L26" s="47" t="s">
         <v>66</v>
       </c>
-      <c r="M26" s="8" t="s">
+      <c r="M26" s="47" t="s">
         <v>186</v>
       </c>
-      <c r="N26" s="8" t="s">
+      <c r="N26" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O26" s="16"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="16" t="s">
+      <c r="O26" s="47"/>
+      <c r="P26" s="47"/>
+      <c r="Q26" s="47"/>
+      <c r="R26" s="47"/>
+      <c r="S26" s="47" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="27" spans="2:20" ht="185.25" x14ac:dyDescent="0.3">
-      <c r="B27" s="45"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="16" t="s">
+      <c r="U26" s="49"/>
+    </row>
+    <row r="27" spans="2:21" s="48" customFormat="1" ht="185.25" x14ac:dyDescent="0.3">
+      <c r="B27" s="38"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="47" t="s">
         <v>303</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="J27" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="K27" s="8" t="s">
+      <c r="K27" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="L27" s="8" t="s">
+      <c r="L27" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="M27" s="8" t="s">
+      <c r="M27" s="47" t="s">
         <v>181</v>
       </c>
-      <c r="N27" s="8" t="s">
+      <c r="N27" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="O27" s="16"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="16" t="s">
+      <c r="O27" s="47"/>
+      <c r="P27" s="47"/>
+      <c r="Q27" s="47"/>
+      <c r="R27" s="47"/>
+      <c r="S27" s="47" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="28" spans="2:20" ht="128.25" x14ac:dyDescent="0.3">
-      <c r="B28" s="45"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="17" t="s">
+      <c r="U27" s="49"/>
+    </row>
+    <row r="28" spans="2:21" s="48" customFormat="1" ht="128.25" x14ac:dyDescent="0.3">
+      <c r="B28" s="38"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="J28" s="47" t="s">
         <v>164</v>
       </c>
-      <c r="K28" s="19" t="s">
+      <c r="K28" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="L28" s="19" t="s">
+      <c r="L28" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="M28" s="19" t="s">
+      <c r="M28" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="N28" s="8" t="s">
+      <c r="N28" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="O28" s="17"/>
-      <c r="P28" s="12"/>
-      <c r="Q28" s="12"/>
-      <c r="R28" s="12"/>
-      <c r="S28" s="17" t="s">
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="29" spans="2:20" ht="102" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="45"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="36" t="s">
+      <c r="U28" s="49"/>
+    </row>
+    <row r="29" spans="2:21" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="38"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="26" t="s">
+      <c r="E29" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="G29" s="26" t="s">
+      <c r="G29" s="31" t="s">
         <v>332</v>
       </c>
-      <c r="H29" s="36" t="s">
+      <c r="H29" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="I29" s="31" t="s">
         <v>304</v>
       </c>
       <c r="J29" s="8" t="s">
@@ -3017,15 +3060,15 @@
         <v>197</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="99.75" x14ac:dyDescent="0.3">
-      <c r="B30" s="45"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="26"/>
+    <row r="30" spans="2:21" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="B30" s="38"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="30"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="31"/>
       <c r="J30" s="8" t="s">
         <v>192</v>
       </c>
@@ -3055,13 +3098,13 @@
         <v>305</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="142.5" x14ac:dyDescent="0.3">
-      <c r="B31" s="45"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="26"/>
+    <row r="31" spans="2:21" ht="142.5" x14ac:dyDescent="0.3">
+      <c r="B31" s="38"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="31"/>
       <c r="H31" s="16" t="s">
         <v>68</v>
       </c>
@@ -3091,13 +3134,13 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="42.75" x14ac:dyDescent="0.3">
-      <c r="B32" s="45"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="26"/>
+    <row r="32" spans="2:21" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="B32" s="38"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
       <c r="H32" s="16" t="s">
         <v>69</v>
       </c>
@@ -3128,12 +3171,12 @@
       </c>
     </row>
     <row r="33" spans="2:19" ht="85.5" x14ac:dyDescent="0.3">
-      <c r="B33" s="45"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="26"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
       <c r="H33" s="16" t="s">
         <v>70</v>
       </c>
@@ -3164,14 +3207,14 @@
       </c>
     </row>
     <row r="34" spans="2:19" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="45"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="36" t="s">
+      <c r="B34" s="38"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="30" t="s">
         <v>413</v>
       </c>
-      <c r="G34" s="26" t="s">
+      <c r="G34" s="31" t="s">
         <v>327</v>
       </c>
       <c r="H34" s="16" t="s">
@@ -3204,12 +3247,12 @@
       </c>
     </row>
     <row r="35" spans="2:19" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="45"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="26"/>
+      <c r="B35" s="38"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="31"/>
       <c r="H35" s="16" t="s">
         <v>314</v>
       </c>
@@ -3240,12 +3283,12 @@
       </c>
     </row>
     <row r="36" spans="2:19" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="45"/>
-      <c r="C36" s="26"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="26"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="31"/>
       <c r="H36" s="15" t="s">
         <v>201</v>
       </c>
@@ -3276,14 +3319,14 @@
       </c>
     </row>
     <row r="37" spans="2:19" ht="128.25" x14ac:dyDescent="0.3">
-      <c r="B37" s="45"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27" t="s">
+      <c r="B37" s="38"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="39" t="s">
         <v>322</v>
       </c>
-      <c r="G37" s="30" t="s">
+      <c r="G37" s="42" t="s">
         <v>333</v>
       </c>
       <c r="H37" s="16" t="s">
@@ -3316,12 +3359,12 @@
       </c>
     </row>
     <row r="38" spans="2:19" ht="128.25" x14ac:dyDescent="0.3">
-      <c r="B38" s="45"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="28"/>
-      <c r="G38" s="31"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="43"/>
       <c r="H38" s="16" t="s">
         <v>78</v>
       </c>
@@ -3352,12 +3395,12 @@
       </c>
     </row>
     <row r="39" spans="2:19" ht="114" x14ac:dyDescent="0.3">
-      <c r="B39" s="45"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="31"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="43"/>
       <c r="H39" s="16" t="s">
         <v>79</v>
       </c>
@@ -3388,12 +3431,12 @@
       </c>
     </row>
     <row r="40" spans="2:19" ht="128.25" x14ac:dyDescent="0.3">
-      <c r="B40" s="45"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="31"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="43"/>
       <c r="H40" s="16" t="s">
         <v>80</v>
       </c>
@@ -3423,17 +3466,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="2:19" ht="57" x14ac:dyDescent="0.3">
-      <c r="B41" s="45"/>
-      <c r="C41" s="26"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="36" t="s">
+    <row r="41" spans="2:19" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="B41" s="38"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="30"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="I41" s="33" t="s">
+      <c r="I41" s="27" t="s">
         <v>331</v>
       </c>
       <c r="J41" s="8" t="s">
@@ -3460,14 +3503,14 @@
       </c>
     </row>
     <row r="42" spans="2:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="45"/>
-      <c r="C42" s="26"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="31"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="47"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="28"/>
       <c r="J42" s="8" t="s">
         <v>198</v>
       </c>
@@ -3492,14 +3535,14 @@
       </c>
     </row>
     <row r="43" spans="2:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="45"/>
-      <c r="C43" s="26"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="31"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="34"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="31"/>
+      <c r="D43" s="30"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="30"/>
+      <c r="I43" s="29"/>
       <c r="J43" s="8" t="s">
         <v>198</v>
       </c>
@@ -3524,12 +3567,12 @@
       </c>
     </row>
     <row r="44" spans="2:19" ht="99.75" x14ac:dyDescent="0.3">
-      <c r="B44" s="45"/>
-      <c r="C44" s="26"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="31"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="43"/>
       <c r="H44" s="16" t="s">
         <v>328</v>
       </c>
@@ -3560,16 +3603,16 @@
       </c>
     </row>
     <row r="45" spans="2:19" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="45"/>
-      <c r="C45" s="26"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="28"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="36" t="s">
+      <c r="B45" s="38"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="I45" s="26" t="s">
+      <c r="I45" s="31" t="s">
         <v>321</v>
       </c>
       <c r="J45" s="8" t="s">
@@ -3596,14 +3639,14 @@
       </c>
     </row>
     <row r="46" spans="2:19" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="45"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="26" t="s">
+      <c r="B46" s="38"/>
+      <c r="C46" s="31"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="31" t="s">
         <v>320</v>
       </c>
       <c r="J46" s="8" t="s">
@@ -3630,12 +3673,12 @@
       </c>
     </row>
     <row r="47" spans="2:19" ht="156.75" x14ac:dyDescent="0.3">
-      <c r="B47" s="45"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="31"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="31"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="43"/>
       <c r="H47" s="16" t="s">
         <v>323</v>
       </c>
@@ -3666,16 +3709,16 @@
       </c>
     </row>
     <row r="48" spans="2:19" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="45"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="31"/>
-      <c r="H48" s="36" t="s">
+      <c r="B48" s="38"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="I48" s="33" t="s">
+      <c r="I48" s="27" t="s">
         <v>334</v>
       </c>
       <c r="J48" s="19" t="s">
@@ -3701,15 +3744,15 @@
         <v>223</v>
       </c>
     </row>
-    <row r="49" spans="2:19" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="45"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="47"/>
+    <row r="49" spans="2:21" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="38"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="30"/>
+      <c r="I49" s="28"/>
       <c r="J49" s="19" t="s">
         <v>221</v>
       </c>
@@ -3733,15 +3776,15 @@
         <v>351</v>
       </c>
     </row>
-    <row r="50" spans="2:19" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="45"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="34"/>
+    <row r="50" spans="2:21" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="38"/>
+      <c r="C50" s="31"/>
+      <c r="D50" s="30"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="41"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="30"/>
+      <c r="I50" s="29"/>
       <c r="J50" s="19" t="s">
         <v>221</v>
       </c>
@@ -3765,1016 +3808,1115 @@
         <v>350</v>
       </c>
     </row>
-    <row r="51" spans="2:19" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="45"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="36" t="s">
+    <row r="51" spans="2:21" s="48" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="38"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="E51" s="26" t="s">
+      <c r="E51" s="45" t="s">
         <v>225</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F51" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="G51" s="26" t="s">
+      <c r="G51" s="45" t="s">
         <v>335</v>
       </c>
-      <c r="H51" s="37" t="s">
+      <c r="H51" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="I51" s="38" t="s">
+      <c r="I51" s="51" t="s">
         <v>338</v>
       </c>
-      <c r="J51" s="46" t="s">
+      <c r="J51" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="K51" s="46" t="s">
+      <c r="K51" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="L51" s="46" t="s">
+      <c r="L51" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="M51" s="46" t="s">
+      <c r="M51" s="51" t="s">
         <v>229</v>
       </c>
-      <c r="N51" s="46" t="s">
+      <c r="N51" s="51" t="s">
         <v>230</v>
       </c>
-      <c r="O51" s="17"/>
-      <c r="P51" s="12"/>
-      <c r="Q51" s="12"/>
-      <c r="R51" s="12"/>
-      <c r="S51" s="17" t="s">
+      <c r="O51" s="50"/>
+      <c r="P51" s="50"/>
+      <c r="Q51" s="50"/>
+      <c r="R51" s="50"/>
+      <c r="S51" s="50" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="52" spans="2:19" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B52" s="45"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="46"/>
-      <c r="K52" s="46"/>
-      <c r="L52" s="46"/>
-      <c r="M52" s="46"/>
-      <c r="N52" s="46"/>
-      <c r="O52" s="17"/>
-      <c r="P52" s="12"/>
-      <c r="Q52" s="12"/>
-      <c r="R52" s="12"/>
-      <c r="S52" s="17" t="s">
+      <c r="U51" s="49"/>
+    </row>
+    <row r="52" spans="2:21" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B52" s="38"/>
+      <c r="C52" s="31"/>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="45"/>
+      <c r="H52" s="51"/>
+      <c r="I52" s="51"/>
+      <c r="J52" s="51"/>
+      <c r="K52" s="51"/>
+      <c r="L52" s="51"/>
+      <c r="M52" s="51"/>
+      <c r="N52" s="51"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="50"/>
+      <c r="Q52" s="50"/>
+      <c r="R52" s="50"/>
+      <c r="S52" s="50" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B53" s="45"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="46"/>
-      <c r="K53" s="46"/>
-      <c r="L53" s="46"/>
-      <c r="M53" s="46"/>
-      <c r="N53" s="46"/>
-      <c r="O53" s="17"/>
-      <c r="P53" s="12"/>
-      <c r="Q53" s="12"/>
-      <c r="R53" s="12"/>
-      <c r="S53" s="17" t="s">
+      <c r="U52" s="49"/>
+    </row>
+    <row r="53" spans="2:21" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="38"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="51"/>
+      <c r="I53" s="51"/>
+      <c r="J53" s="51"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="51"/>
+      <c r="M53" s="51"/>
+      <c r="N53" s="51"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="50"/>
+      <c r="Q53" s="50"/>
+      <c r="R53" s="50"/>
+      <c r="S53" s="50" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="54" spans="2:19" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B54" s="45"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="26"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="46"/>
-      <c r="K54" s="46"/>
-      <c r="L54" s="46"/>
-      <c r="M54" s="46"/>
-      <c r="N54" s="46"/>
-      <c r="O54" s="17"/>
-      <c r="P54" s="12"/>
-      <c r="Q54" s="12"/>
-      <c r="R54" s="12"/>
-      <c r="S54" s="17" t="s">
+      <c r="U53" s="49"/>
+    </row>
+    <row r="54" spans="2:21" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B54" s="38"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="51"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="51"/>
+      <c r="N54" s="51"/>
+      <c r="O54" s="50"/>
+      <c r="P54" s="50"/>
+      <c r="Q54" s="50"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="55" spans="2:19" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="45"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="37" t="s">
+      <c r="U54" s="49"/>
+    </row>
+    <row r="55" spans="2:21" s="48" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B55" s="38"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="51" t="s">
         <v>92</v>
       </c>
-      <c r="I55" s="38" t="s">
+      <c r="I55" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="J55" s="46" t="s">
+      <c r="J55" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="K55" s="46" t="s">
+      <c r="K55" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="L55" s="46" t="s">
+      <c r="L55" s="51" t="s">
         <v>231</v>
       </c>
-      <c r="M55" s="46" t="s">
+      <c r="M55" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="N55" s="46" t="s">
+      <c r="N55" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="O55" s="17"/>
-      <c r="P55" s="12"/>
-      <c r="Q55" s="12"/>
-      <c r="R55" s="12"/>
-      <c r="S55" s="17" t="s">
+      <c r="O55" s="50"/>
+      <c r="P55" s="50"/>
+      <c r="Q55" s="50"/>
+      <c r="R55" s="50"/>
+      <c r="S55" s="50" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="56" spans="2:19" ht="42" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="45"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="37"/>
-      <c r="I56" s="38"/>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-      <c r="N56" s="46"/>
-      <c r="O56" s="17"/>
-      <c r="P56" s="12"/>
-      <c r="Q56" s="12"/>
-      <c r="R56" s="12"/>
-      <c r="S56" s="16" t="s">
+      <c r="U55" s="49"/>
+    </row>
+    <row r="56" spans="2:21" s="48" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="38"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="51"/>
+      <c r="I56" s="51"/>
+      <c r="J56" s="51"/>
+      <c r="K56" s="51"/>
+      <c r="L56" s="51"/>
+      <c r="M56" s="51"/>
+      <c r="N56" s="51"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="50"/>
+      <c r="Q56" s="50"/>
+      <c r="R56" s="50"/>
+      <c r="S56" s="47" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="57" spans="2:19" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="45"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="37" t="s">
+      <c r="U56" s="49"/>
+    </row>
+    <row r="57" spans="2:21" s="48" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="38"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="I57" s="38" t="s">
+      <c r="I57" s="51" t="s">
         <v>341</v>
       </c>
-      <c r="J57" s="46" t="s">
+      <c r="J57" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="K57" s="46" t="s">
+      <c r="K57" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="L57" s="46" t="s">
+      <c r="L57" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="M57" s="46" t="s">
+      <c r="M57" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="N57" s="46" t="s">
+      <c r="N57" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="O57" s="17"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="17" t="s">
+      <c r="O57" s="50"/>
+      <c r="P57" s="50"/>
+      <c r="Q57" s="50"/>
+      <c r="R57" s="50"/>
+      <c r="S57" s="50" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="58" spans="2:19" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="45"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="26"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="38"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-      <c r="N58" s="46"/>
-      <c r="O58" s="17"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="16" t="s">
+      <c r="U57" s="49"/>
+    </row>
+    <row r="58" spans="2:21" s="48" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="38"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="51"/>
+      <c r="I58" s="51"/>
+      <c r="J58" s="51"/>
+      <c r="K58" s="51"/>
+      <c r="L58" s="51"/>
+      <c r="M58" s="51"/>
+      <c r="N58" s="51"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="50"/>
+      <c r="Q58" s="50"/>
+      <c r="R58" s="50"/>
+      <c r="S58" s="47" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="59" spans="2:19" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="45"/>
-      <c r="C59" s="26"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="37" t="s">
+      <c r="U58" s="49"/>
+    </row>
+    <row r="59" spans="2:21" s="48" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B59" s="38"/>
+      <c r="C59" s="31"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="I59" s="38" t="s">
+      <c r="I59" s="51" t="s">
         <v>344</v>
       </c>
-      <c r="J59" s="46" t="s">
+      <c r="J59" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="K59" s="46" t="s">
+      <c r="K59" s="51" t="s">
         <v>228</v>
       </c>
-      <c r="L59" s="46" t="s">
+      <c r="L59" s="51" t="s">
         <v>233</v>
       </c>
-      <c r="M59" s="46" t="s">
+      <c r="M59" s="51" t="s">
         <v>343</v>
       </c>
-      <c r="N59" s="46" t="s">
+      <c r="N59" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="O59" s="17"/>
-      <c r="P59" s="12"/>
-      <c r="Q59" s="12"/>
-      <c r="R59" s="12"/>
-      <c r="S59" s="17" t="s">
+      <c r="O59" s="50"/>
+      <c r="P59" s="50"/>
+      <c r="Q59" s="50"/>
+      <c r="R59" s="50"/>
+      <c r="S59" s="50" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="60" spans="2:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="45"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="37"/>
-      <c r="I60" s="38"/>
-      <c r="J60" s="46"/>
-      <c r="K60" s="46"/>
-      <c r="L60" s="46"/>
-      <c r="M60" s="46"/>
-      <c r="N60" s="46"/>
-      <c r="O60" s="17"/>
-      <c r="P60" s="12"/>
-      <c r="Q60" s="12"/>
-      <c r="R60" s="12"/>
-      <c r="S60" s="17" t="s">
+      <c r="U59" s="49"/>
+    </row>
+    <row r="60" spans="2:21" s="48" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B60" s="38"/>
+      <c r="C60" s="31"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="45"/>
+      <c r="H60" s="51"/>
+      <c r="I60" s="51"/>
+      <c r="J60" s="51"/>
+      <c r="K60" s="51"/>
+      <c r="L60" s="51"/>
+      <c r="M60" s="51"/>
+      <c r="N60" s="51"/>
+      <c r="O60" s="50"/>
+      <c r="P60" s="50"/>
+      <c r="Q60" s="50"/>
+      <c r="R60" s="50"/>
+      <c r="S60" s="50" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="61" spans="2:19" ht="99.75" x14ac:dyDescent="0.3">
-      <c r="B61" s="45"/>
-      <c r="C61" s="26"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="26"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="17" t="s">
+      <c r="U60" s="49"/>
+    </row>
+    <row r="61" spans="2:21" s="48" customFormat="1" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="B61" s="38"/>
+      <c r="C61" s="31"/>
+      <c r="D61" s="45"/>
+      <c r="E61" s="45"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="I61" s="12" t="s">
+      <c r="I61" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="J61" s="19" t="s">
+      <c r="J61" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="K61" s="19" t="s">
+      <c r="K61" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="L61" s="19" t="s">
+      <c r="L61" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="M61" s="19" t="s">
+      <c r="M61" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="N61" s="19" t="s">
+      <c r="N61" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O61" s="17"/>
-      <c r="P61" s="12"/>
-      <c r="Q61" s="12"/>
-      <c r="R61" s="12"/>
-      <c r="S61" s="17" t="s">
+      <c r="O61" s="50"/>
+      <c r="P61" s="50"/>
+      <c r="Q61" s="50"/>
+      <c r="R61" s="50"/>
+      <c r="S61" s="50" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="62" spans="2:19" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="45"/>
-      <c r="C62" s="26"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="26"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="37" t="s">
+      <c r="U61" s="49"/>
+    </row>
+    <row r="62" spans="2:21" s="48" customFormat="1" ht="84.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="38"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="45"/>
+      <c r="E62" s="45"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="45"/>
+      <c r="H62" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="I62" s="38" t="s">
+      <c r="I62" s="51" t="s">
         <v>129</v>
       </c>
-      <c r="J62" s="46" t="s">
+      <c r="J62" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="K62" s="46" t="s">
+      <c r="K62" s="51" t="s">
         <v>234</v>
       </c>
-      <c r="L62" s="46" t="s">
+      <c r="L62" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="M62" s="46" t="s">
+      <c r="M62" s="51" t="s">
         <v>235</v>
       </c>
-      <c r="N62" s="46" t="s">
+      <c r="N62" s="51" t="s">
         <v>232</v>
       </c>
-      <c r="O62" s="17"/>
-      <c r="P62" s="12"/>
-      <c r="Q62" s="12"/>
-      <c r="R62" s="12"/>
-      <c r="S62" s="17" t="s">
+      <c r="O62" s="50"/>
+      <c r="P62" s="50"/>
+      <c r="Q62" s="50"/>
+      <c r="R62" s="50"/>
+      <c r="S62" s="50" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="63" spans="2:19" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="45"/>
-      <c r="C63" s="26"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="26"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="37"/>
-      <c r="I63" s="38"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="46"/>
-      <c r="M63" s="46"/>
-      <c r="N63" s="46"/>
-      <c r="O63" s="17"/>
-      <c r="P63" s="12"/>
-      <c r="Q63" s="12"/>
-      <c r="R63" s="12"/>
-      <c r="S63" s="17" t="s">
+      <c r="U62" s="49"/>
+    </row>
+    <row r="63" spans="2:21" s="48" customFormat="1" ht="109.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="38"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="45"/>
+      <c r="E63" s="45"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="45"/>
+      <c r="H63" s="51"/>
+      <c r="I63" s="51"/>
+      <c r="J63" s="51"/>
+      <c r="K63" s="51"/>
+      <c r="L63" s="51"/>
+      <c r="M63" s="51"/>
+      <c r="N63" s="51"/>
+      <c r="O63" s="50"/>
+      <c r="P63" s="50"/>
+      <c r="Q63" s="50"/>
+      <c r="R63" s="50"/>
+      <c r="S63" s="50" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="64" spans="2:19" ht="114" x14ac:dyDescent="0.3">
-      <c r="B64" s="45"/>
-      <c r="C64" s="26"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="26"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="17" t="s">
+      <c r="U63" s="49"/>
+    </row>
+    <row r="64" spans="2:21" s="48" customFormat="1" ht="114" x14ac:dyDescent="0.3">
+      <c r="B64" s="38"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="45"/>
+      <c r="H64" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="I64" s="12" t="s">
+      <c r="I64" s="50" t="s">
         <v>337</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="J64" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="K64" s="19" t="s">
+      <c r="K64" s="50" t="s">
         <v>234</v>
       </c>
-      <c r="L64" s="19" t="s">
+      <c r="L64" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="M64" s="19" t="s">
+      <c r="M64" s="50" t="s">
         <v>235</v>
       </c>
-      <c r="N64" s="19" t="s">
+      <c r="N64" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O64" s="17"/>
-      <c r="P64" s="12"/>
-      <c r="Q64" s="12"/>
-      <c r="R64" s="12"/>
-      <c r="S64" s="17" t="s">
+      <c r="O64" s="50"/>
+      <c r="P64" s="50"/>
+      <c r="Q64" s="50"/>
+      <c r="R64" s="50"/>
+      <c r="S64" s="50" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="65" spans="2:19" ht="42.75" x14ac:dyDescent="0.3">
-      <c r="B65" s="45"/>
-      <c r="C65" s="26"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="26"/>
-      <c r="F65" s="36"/>
-      <c r="G65" s="26"/>
-      <c r="H65" s="16" t="s">
+      <c r="U64" s="49"/>
+    </row>
+    <row r="65" spans="2:21" s="48" customFormat="1" ht="42.75" x14ac:dyDescent="0.3">
+      <c r="B65" s="38"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="45"/>
+      <c r="E65" s="45"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="45"/>
+      <c r="H65" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="I65" s="11" t="s">
+      <c r="I65" s="47" t="s">
         <v>131</v>
       </c>
-      <c r="J65" s="8" t="s">
+      <c r="J65" s="47" t="s">
         <v>221</v>
       </c>
-      <c r="K65" s="8" t="s">
+      <c r="K65" s="47" t="s">
         <v>248</v>
       </c>
-      <c r="L65" s="8" t="s">
+      <c r="L65" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="M65" s="8" t="s">
+      <c r="M65" s="47" t="s">
         <v>236</v>
       </c>
-      <c r="N65" s="8" t="s">
+      <c r="N65" s="47" t="s">
         <v>224</v>
       </c>
-      <c r="O65" s="16"/>
-      <c r="P65" s="11"/>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="S65" s="17" t="s">
+      <c r="O65" s="47"/>
+      <c r="P65" s="47"/>
+      <c r="Q65" s="47"/>
+      <c r="R65" s="47"/>
+      <c r="S65" s="50" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="66" spans="2:19" ht="216" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="45"/>
-      <c r="C66" s="26"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="26"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="37" t="s">
+      <c r="U65" s="49"/>
+    </row>
+    <row r="66" spans="2:21" s="48" customFormat="1" ht="216" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="38"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="45"/>
+      <c r="H66" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="I66" s="33" t="s">
+      <c r="I66" s="52" t="s">
         <v>345</v>
       </c>
-      <c r="J66" s="19" t="s">
+      <c r="J66" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="K66" s="19" t="s">
+      <c r="K66" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="L66" s="19" t="s">
+      <c r="L66" s="50" t="s">
         <v>245</v>
       </c>
-      <c r="M66" s="19" t="s">
+      <c r="M66" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="N66" s="19" t="s">
+      <c r="N66" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O66" s="17"/>
-      <c r="P66" s="12" t="s">
+      <c r="O66" s="50"/>
+      <c r="P66" s="50" t="s">
         <v>336</v>
       </c>
-      <c r="Q66" s="12"/>
-      <c r="R66" s="12"/>
-      <c r="S66" s="17" t="s">
+      <c r="Q66" s="50"/>
+      <c r="R66" s="50"/>
+      <c r="S66" s="50" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="67" spans="2:19" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="45"/>
-      <c r="C67" s="26"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="26"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="37"/>
-      <c r="I67" s="34"/>
-      <c r="J67" s="19" t="s">
+      <c r="U66" s="49"/>
+    </row>
+    <row r="67" spans="2:21" s="48" customFormat="1" ht="188.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B67" s="38"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="45"/>
+      <c r="H67" s="51"/>
+      <c r="I67" s="53"/>
+      <c r="J67" s="50" t="s">
         <v>247</v>
       </c>
-      <c r="K67" s="19" t="s">
+      <c r="K67" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="L67" s="19" t="s">
+      <c r="L67" s="50" t="s">
         <v>246</v>
       </c>
-      <c r="M67" s="19" t="s">
+      <c r="M67" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="N67" s="19" t="s">
+      <c r="N67" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O67" s="17"/>
-      <c r="P67" s="12" t="s">
+      <c r="O67" s="50"/>
+      <c r="P67" s="50" t="s">
         <v>346</v>
       </c>
-      <c r="Q67" s="12"/>
-      <c r="R67" s="12"/>
-      <c r="S67" s="17" t="s">
+      <c r="Q67" s="50"/>
+      <c r="R67" s="50"/>
+      <c r="S67" s="50" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="68" spans="2:19" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="45"/>
-      <c r="C68" s="26"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="26"/>
-      <c r="F68" s="36" t="s">
+      <c r="U67" s="49"/>
+    </row>
+    <row r="68" spans="2:21" s="48" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="38"/>
+      <c r="C68" s="31"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="45"/>
+      <c r="F68" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="G68" s="26" t="s">
+      <c r="G68" s="45" t="s">
         <v>348</v>
       </c>
-      <c r="H68" s="16" t="s">
+      <c r="H68" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="I68" s="12" t="s">
+      <c r="I68" s="50" t="s">
         <v>347</v>
       </c>
-      <c r="J68" s="19" t="s">
+      <c r="J68" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="K68" s="19" t="s">
+      <c r="K68" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="L68" s="19" t="s">
+      <c r="L68" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="M68" s="51" t="s">
+      <c r="M68" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="N68" s="19" t="s">
+      <c r="N68" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O68" s="17"/>
-      <c r="P68" s="12"/>
-      <c r="Q68" s="12"/>
-      <c r="R68" s="12"/>
-      <c r="S68" s="16" t="s">
+      <c r="O68" s="50"/>
+      <c r="P68" s="50"/>
+      <c r="Q68" s="50"/>
+      <c r="R68" s="50"/>
+      <c r="S68" s="47" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="69" spans="2:19" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="45"/>
-      <c r="C69" s="26"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="26"/>
-      <c r="F69" s="36"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="16" t="s">
+      <c r="U68" s="49"/>
+    </row>
+    <row r="69" spans="2:21" s="48" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="38"/>
+      <c r="C69" s="31"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="I69" s="12" t="s">
+      <c r="I69" s="50" t="s">
         <v>349</v>
       </c>
-      <c r="J69" s="19" t="s">
+      <c r="J69" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="K69" s="19" t="s">
+      <c r="K69" s="50" t="s">
         <v>253</v>
       </c>
-      <c r="L69" s="19" t="s">
+      <c r="L69" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="M69" s="51" t="s">
+      <c r="M69" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="N69" s="19" t="s">
+      <c r="N69" s="50" t="s">
         <v>232</v>
       </c>
-      <c r="O69" s="17"/>
-      <c r="P69" s="12"/>
-      <c r="Q69" s="12"/>
-      <c r="R69" s="12"/>
-      <c r="S69" s="17" t="s">
+      <c r="O69" s="50"/>
+      <c r="P69" s="50"/>
+      <c r="Q69" s="50"/>
+      <c r="R69" s="50"/>
+      <c r="S69" s="50" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="70" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="45"/>
-      <c r="C70" s="26"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="26"/>
-      <c r="F70" s="27" t="s">
+      <c r="U69" s="49"/>
+    </row>
+    <row r="70" spans="2:21" s="48" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="38"/>
+      <c r="C70" s="31"/>
+      <c r="D70" s="45"/>
+      <c r="E70" s="45"/>
+      <c r="F70" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="G70" s="30" t="s">
+      <c r="G70" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="H70" s="37" t="s">
+      <c r="H70" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="I70" s="38" t="s">
+      <c r="I70" s="51" t="s">
         <v>134</v>
       </c>
-      <c r="J70" s="48" t="s">
+      <c r="J70" s="52" t="s">
         <v>254</v>
       </c>
-      <c r="K70" s="48" t="s">
+      <c r="K70" s="52" t="s">
         <v>256</v>
       </c>
-      <c r="L70" s="48" t="s">
+      <c r="L70" s="52" t="s">
         <v>255</v>
       </c>
-      <c r="M70" s="48" t="s">
+      <c r="M70" s="52" t="s">
         <v>257</v>
       </c>
-      <c r="N70" s="48" t="s">
+      <c r="N70" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="O70" s="17"/>
-      <c r="P70" s="12"/>
-      <c r="Q70" s="12"/>
-      <c r="R70" s="12"/>
-      <c r="S70" s="17" t="s">
+      <c r="O70" s="50"/>
+      <c r="P70" s="50"/>
+      <c r="Q70" s="50"/>
+      <c r="R70" s="50"/>
+      <c r="S70" s="50" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="71" spans="2:19" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B71" s="45"/>
-      <c r="C71" s="26"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="26"/>
-      <c r="F71" s="28"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="37"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="50"/>
-      <c r="K71" s="50"/>
-      <c r="L71" s="50"/>
-      <c r="M71" s="50"/>
-      <c r="N71" s="50"/>
-      <c r="O71" s="17"/>
-      <c r="P71" s="12"/>
-      <c r="Q71" s="12"/>
-      <c r="R71" s="12"/>
-      <c r="S71" s="17" t="s">
+      <c r="U70" s="49"/>
+    </row>
+    <row r="71" spans="2:21" s="48" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B71" s="38"/>
+      <c r="C71" s="31"/>
+      <c r="D71" s="45"/>
+      <c r="E71" s="45"/>
+      <c r="F71" s="55"/>
+      <c r="G71" s="55"/>
+      <c r="H71" s="51"/>
+      <c r="I71" s="51"/>
+      <c r="J71" s="56"/>
+      <c r="K71" s="56"/>
+      <c r="L71" s="56"/>
+      <c r="M71" s="56"/>
+      <c r="N71" s="56"/>
+      <c r="O71" s="50"/>
+      <c r="P71" s="50"/>
+      <c r="Q71" s="50"/>
+      <c r="R71" s="50"/>
+      <c r="S71" s="50" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="72" spans="2:19" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="45"/>
-      <c r="C72" s="26"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="26"/>
-      <c r="F72" s="28"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="37"/>
-      <c r="I72" s="38"/>
-      <c r="J72" s="50"/>
-      <c r="K72" s="50"/>
-      <c r="L72" s="50"/>
-      <c r="M72" s="50"/>
-      <c r="N72" s="50"/>
-      <c r="O72" s="17"/>
-      <c r="P72" s="12"/>
-      <c r="Q72" s="12"/>
-      <c r="R72" s="12"/>
-      <c r="S72" s="17" t="s">
+      <c r="U71" s="49"/>
+    </row>
+    <row r="72" spans="2:21" s="48" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="38"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="45"/>
+      <c r="E72" s="45"/>
+      <c r="F72" s="55"/>
+      <c r="G72" s="55"/>
+      <c r="H72" s="51"/>
+      <c r="I72" s="51"/>
+      <c r="J72" s="56"/>
+      <c r="K72" s="56"/>
+      <c r="L72" s="56"/>
+      <c r="M72" s="56"/>
+      <c r="N72" s="56"/>
+      <c r="O72" s="50"/>
+      <c r="P72" s="50"/>
+      <c r="Q72" s="50"/>
+      <c r="R72" s="50"/>
+      <c r="S72" s="50" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="73" spans="2:19" ht="57" x14ac:dyDescent="0.3">
-      <c r="B73" s="45"/>
-      <c r="C73" s="26"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="28"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="37"/>
-      <c r="I73" s="38"/>
-      <c r="J73" s="49"/>
-      <c r="K73" s="49"/>
-      <c r="L73" s="49"/>
-      <c r="M73" s="49"/>
-      <c r="N73" s="49"/>
-      <c r="O73" s="17"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="12"/>
-      <c r="R73" s="12"/>
-      <c r="S73" s="17" t="s">
+      <c r="U72" s="49"/>
+    </row>
+    <row r="73" spans="2:21" s="48" customFormat="1" ht="57" x14ac:dyDescent="0.3">
+      <c r="B73" s="38"/>
+      <c r="C73" s="31"/>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
+      <c r="F73" s="55"/>
+      <c r="G73" s="55"/>
+      <c r="H73" s="51"/>
+      <c r="I73" s="51"/>
+      <c r="J73" s="53"/>
+      <c r="K73" s="53"/>
+      <c r="L73" s="53"/>
+      <c r="M73" s="53"/>
+      <c r="N73" s="53"/>
+      <c r="O73" s="50"/>
+      <c r="P73" s="50"/>
+      <c r="Q73" s="50"/>
+      <c r="R73" s="50"/>
+      <c r="S73" s="50" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="74" spans="2:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="45"/>
-      <c r="C74" s="26"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="26"/>
-      <c r="F74" s="28"/>
-      <c r="G74" s="31"/>
-      <c r="H74" s="27" t="s">
+      <c r="U73" s="49"/>
+    </row>
+    <row r="74" spans="2:21" s="48" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B74" s="38"/>
+      <c r="C74" s="31"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+      <c r="F74" s="55"/>
+      <c r="G74" s="55"/>
+      <c r="H74" s="54" t="s">
         <v>414</v>
       </c>
-      <c r="I74" s="26" t="s">
+      <c r="I74" s="45" t="s">
         <v>360</v>
       </c>
-      <c r="J74" s="48" t="s">
+      <c r="J74" s="52" t="s">
         <v>357</v>
       </c>
-      <c r="K74" s="48" t="s">
+      <c r="K74" s="52" t="s">
         <v>266</v>
       </c>
-      <c r="L74" s="35" t="s">
+      <c r="L74" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="M74" s="19" t="s">
+      <c r="M74" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="N74" s="48" t="s">
+      <c r="N74" s="52" t="s">
         <v>361</v>
       </c>
-      <c r="O74" s="17"/>
-      <c r="P74" s="12"/>
-      <c r="Q74" s="12"/>
-      <c r="R74" s="12"/>
-      <c r="S74" s="17" t="s">
+      <c r="O74" s="50"/>
+      <c r="P74" s="50"/>
+      <c r="Q74" s="50"/>
+      <c r="R74" s="50"/>
+      <c r="S74" s="50" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="75" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="45"/>
-      <c r="C75" s="26"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="26"/>
-      <c r="F75" s="28"/>
-      <c r="G75" s="31"/>
-      <c r="H75" s="28"/>
-      <c r="I75" s="26"/>
-      <c r="J75" s="49"/>
-      <c r="K75" s="49"/>
-      <c r="L75" s="35"/>
-      <c r="M75" s="19" t="s">
+      <c r="U74" s="49"/>
+    </row>
+    <row r="75" spans="2:21" s="48" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="38"/>
+      <c r="C75" s="31"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="55"/>
+      <c r="G75" s="55"/>
+      <c r="H75" s="55"/>
+      <c r="I75" s="45"/>
+      <c r="J75" s="53"/>
+      <c r="K75" s="53"/>
+      <c r="L75" s="45"/>
+      <c r="M75" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="N75" s="49"/>
-      <c r="O75" s="17"/>
-      <c r="P75" s="12"/>
-      <c r="Q75" s="12"/>
-      <c r="R75" s="12"/>
-      <c r="S75" s="16" t="s">
+      <c r="N75" s="53"/>
+      <c r="O75" s="50"/>
+      <c r="P75" s="50"/>
+      <c r="Q75" s="50"/>
+      <c r="R75" s="50"/>
+      <c r="S75" s="47" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="76" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="45"/>
-      <c r="C76" s="26"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="26"/>
-      <c r="F76" s="28"/>
-      <c r="G76" s="31"/>
-      <c r="H76" s="28"/>
-      <c r="I76" s="26"/>
-      <c r="J76" s="48" t="s">
+      <c r="U75" s="49"/>
+    </row>
+    <row r="76" spans="2:21" s="48" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="38"/>
+      <c r="C76" s="31"/>
+      <c r="D76" s="45"/>
+      <c r="E76" s="45"/>
+      <c r="F76" s="55"/>
+      <c r="G76" s="55"/>
+      <c r="H76" s="55"/>
+      <c r="I76" s="45"/>
+      <c r="J76" s="52" t="s">
         <v>358</v>
       </c>
-      <c r="K76" s="48" t="s">
+      <c r="K76" s="52" t="s">
         <v>266</v>
       </c>
-      <c r="L76" s="46" t="s">
+      <c r="L76" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="M76" s="19" t="s">
+      <c r="M76" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="N76" s="48" t="s">
+      <c r="N76" s="52" t="s">
         <v>361</v>
       </c>
-      <c r="O76" s="17"/>
-      <c r="P76" s="12"/>
-      <c r="Q76" s="12"/>
-      <c r="R76" s="12"/>
-      <c r="S76" s="17" t="s">
+      <c r="O76" s="50"/>
+      <c r="P76" s="50"/>
+      <c r="Q76" s="50"/>
+      <c r="R76" s="50"/>
+      <c r="S76" s="50" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="77" spans="2:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B77" s="45"/>
-      <c r="C77" s="26"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="26"/>
-      <c r="F77" s="28"/>
-      <c r="G77" s="31"/>
-      <c r="H77" s="28"/>
-      <c r="I77" s="26"/>
-      <c r="J77" s="50"/>
-      <c r="K77" s="50"/>
-      <c r="L77" s="46"/>
-      <c r="M77" s="19" t="s">
+      <c r="U76" s="49"/>
+    </row>
+    <row r="77" spans="2:21" s="48" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B77" s="38"/>
+      <c r="C77" s="31"/>
+      <c r="D77" s="45"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="55"/>
+      <c r="G77" s="55"/>
+      <c r="H77" s="55"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="56"/>
+      <c r="K77" s="56"/>
+      <c r="L77" s="51"/>
+      <c r="M77" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="N77" s="50"/>
-      <c r="O77" s="17"/>
-      <c r="P77" s="12"/>
-      <c r="Q77" s="12"/>
-      <c r="R77" s="12"/>
-      <c r="S77" s="17" t="s">
+      <c r="N77" s="56"/>
+      <c r="O77" s="50"/>
+      <c r="P77" s="50"/>
+      <c r="Q77" s="50"/>
+      <c r="R77" s="50"/>
+      <c r="S77" s="50" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="78" spans="2:19" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B78" s="45"/>
-      <c r="C78" s="26"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="26"/>
-      <c r="F78" s="28"/>
-      <c r="G78" s="31"/>
-      <c r="H78" s="28"/>
-      <c r="I78" s="26"/>
-      <c r="J78" s="19" t="s">
+      <c r="U77" s="49"/>
+    </row>
+    <row r="78" spans="2:21" s="48" customFormat="1" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B78" s="38"/>
+      <c r="C78" s="31"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="55"/>
+      <c r="G78" s="55"/>
+      <c r="H78" s="55"/>
+      <c r="I78" s="45"/>
+      <c r="J78" s="50" t="s">
         <v>359</v>
       </c>
-      <c r="K78" s="19" t="s">
+      <c r="K78" s="50" t="s">
         <v>266</v>
       </c>
-      <c r="L78" s="19" t="s">
+      <c r="L78" s="50" t="s">
         <v>264</v>
       </c>
-      <c r="M78" s="19" t="s">
+      <c r="M78" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="N78" s="48" t="s">
+      <c r="N78" s="52" t="s">
         <v>230</v>
       </c>
-      <c r="O78" s="17"/>
-      <c r="P78" s="12"/>
-      <c r="Q78" s="12"/>
-      <c r="R78" s="12"/>
-      <c r="S78" s="17" t="s">
+      <c r="O78" s="50"/>
+      <c r="P78" s="50"/>
+      <c r="Q78" s="50"/>
+      <c r="R78" s="50"/>
+      <c r="S78" s="50" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="79" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B79" s="45"/>
-      <c r="C79" s="26"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="26"/>
-      <c r="F79" s="29"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="29"/>
-      <c r="I79" s="26"/>
-      <c r="J79" s="19" t="s">
+      <c r="U78" s="49"/>
+    </row>
+    <row r="79" spans="2:21" s="48" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="38"/>
+      <c r="C79" s="31"/>
+      <c r="D79" s="45"/>
+      <c r="E79" s="45"/>
+      <c r="F79" s="57"/>
+      <c r="G79" s="57"/>
+      <c r="H79" s="57"/>
+      <c r="I79" s="45"/>
+      <c r="J79" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="K79" s="19" t="s">
+      <c r="K79" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="L79" s="19" t="s">
+      <c r="L79" s="50" t="s">
         <v>265</v>
       </c>
-      <c r="M79" s="19" t="s">
+      <c r="M79" s="50" t="s">
         <v>272</v>
       </c>
-      <c r="N79" s="49"/>
-      <c r="O79" s="17"/>
-      <c r="P79" s="12"/>
-      <c r="Q79" s="12"/>
-      <c r="R79" s="12"/>
-      <c r="S79" s="17" t="s">
+      <c r="N79" s="53"/>
+      <c r="O79" s="50"/>
+      <c r="P79" s="50"/>
+      <c r="Q79" s="50"/>
+      <c r="R79" s="50"/>
+      <c r="S79" s="50" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="80" spans="2:19" ht="71.25" x14ac:dyDescent="0.3">
-      <c r="B80" s="45"/>
-      <c r="C80" s="26"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="26"/>
-      <c r="F80" s="36" t="s">
+      <c r="U79" s="49"/>
+    </row>
+    <row r="80" spans="2:21" s="48" customFormat="1" ht="71.25" x14ac:dyDescent="0.3">
+      <c r="B80" s="38"/>
+      <c r="C80" s="31"/>
+      <c r="D80" s="45"/>
+      <c r="E80" s="45"/>
+      <c r="F80" s="45" t="s">
         <v>352</v>
       </c>
-      <c r="G80" s="26" t="s">
+      <c r="G80" s="45" t="s">
         <v>353</v>
       </c>
-      <c r="H80" s="16" t="s">
+      <c r="H80" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="I80" s="11" t="s">
+      <c r="I80" s="47" t="s">
         <v>132</v>
       </c>
-      <c r="J80" s="8" t="s">
+      <c r="J80" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="K80" s="8" t="s">
+      <c r="K80" s="47" t="s">
         <v>273</v>
       </c>
-      <c r="L80" s="8" t="s">
+      <c r="L80" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="M80" s="8" t="s">
+      <c r="M80" s="47" t="s">
         <v>274</v>
       </c>
-      <c r="N80" s="8" t="s">
+      <c r="N80" s="47" t="s">
         <v>275</v>
       </c>
-      <c r="O80" s="16"/>
-      <c r="P80" s="11"/>
-      <c r="Q80" s="11"/>
-      <c r="R80" s="11"/>
-      <c r="S80" s="16" t="s">
+      <c r="O80" s="47"/>
+      <c r="P80" s="47"/>
+      <c r="Q80" s="47"/>
+      <c r="R80" s="47"/>
+      <c r="S80" s="47" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="81" spans="2:19" ht="114" x14ac:dyDescent="0.3">
-      <c r="B81" s="45"/>
-      <c r="C81" s="26"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="26"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="16" t="s">
+      <c r="U80" s="49"/>
+    </row>
+    <row r="81" spans="2:21" s="48" customFormat="1" ht="114" x14ac:dyDescent="0.3">
+      <c r="B81" s="38"/>
+      <c r="C81" s="31"/>
+      <c r="D81" s="45"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="45"/>
+      <c r="G81" s="45"/>
+      <c r="H81" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="I81" s="11" t="s">
+      <c r="I81" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="J81" s="8" t="s">
+      <c r="J81" s="47" t="s">
         <v>198</v>
       </c>
-      <c r="K81" s="8" t="s">
+      <c r="K81" s="47" t="s">
         <v>276</v>
       </c>
-      <c r="L81" s="8" t="s">
+      <c r="L81" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="M81" s="8" t="s">
+      <c r="M81" s="47" t="s">
         <v>114</v>
       </c>
-      <c r="N81" s="8" t="s">
+      <c r="N81" s="47" t="s">
         <v>277</v>
       </c>
-      <c r="O81" s="16"/>
-      <c r="P81" s="11"/>
-      <c r="Q81" s="11"/>
-      <c r="R81" s="11"/>
-      <c r="S81" s="16" t="s">
+      <c r="O81" s="47"/>
+      <c r="P81" s="47"/>
+      <c r="Q81" s="47"/>
+      <c r="R81" s="47"/>
+      <c r="S81" s="47" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="82" spans="2:19" ht="99.75" x14ac:dyDescent="0.3">
-      <c r="B82" s="45"/>
-      <c r="C82" s="26"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="26"/>
-      <c r="F82" s="36"/>
-      <c r="G82" s="26"/>
-      <c r="H82" s="16" t="s">
+      <c r="U81" s="49"/>
+    </row>
+    <row r="82" spans="2:21" s="48" customFormat="1" ht="99.75" x14ac:dyDescent="0.3">
+      <c r="B82" s="38"/>
+      <c r="C82" s="31"/>
+      <c r="D82" s="45"/>
+      <c r="E82" s="45"/>
+      <c r="F82" s="45"/>
+      <c r="G82" s="45"/>
+      <c r="H82" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="I82" s="11" t="s">
+      <c r="I82" s="47" t="s">
         <v>356</v>
       </c>
-      <c r="J82" s="8" t="s">
+      <c r="J82" s="47" t="s">
         <v>278</v>
       </c>
-      <c r="K82" s="8" t="s">
+      <c r="K82" s="47" t="s">
         <v>279</v>
       </c>
-      <c r="L82" s="8" t="s">
+      <c r="L82" s="47" t="s">
         <v>354</v>
       </c>
-      <c r="M82" s="8" t="s">
+      <c r="M82" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="N82" s="8" t="s">
+      <c r="N82" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="O82" s="16"/>
-      <c r="P82" s="11"/>
-      <c r="Q82" s="11"/>
-      <c r="R82" s="11"/>
-      <c r="S82" s="16" t="s">
+      <c r="O82" s="47"/>
+      <c r="P82" s="47"/>
+      <c r="Q82" s="47"/>
+      <c r="R82" s="47"/>
+      <c r="S82" s="47" t="s">
         <v>355</v>
       </c>
+      <c r="U82" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="119">
-    <mergeCell ref="N78:N79"/>
-    <mergeCell ref="J74:J75"/>
-    <mergeCell ref="K74:K75"/>
-    <mergeCell ref="J76:J77"/>
-    <mergeCell ref="K76:K77"/>
-    <mergeCell ref="N70:N73"/>
-    <mergeCell ref="L74:L75"/>
-    <mergeCell ref="L76:L77"/>
-    <mergeCell ref="N74:N75"/>
-    <mergeCell ref="N76:N77"/>
-    <mergeCell ref="J70:J73"/>
-    <mergeCell ref="L70:L73"/>
-    <mergeCell ref="K70:K73"/>
-    <mergeCell ref="M70:M73"/>
+    <mergeCell ref="E13:E28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="F37:F50"/>
+    <mergeCell ref="G37:G50"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="F70:F79"/>
+    <mergeCell ref="G70:G79"/>
+    <mergeCell ref="H74:H79"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="E51:E82"/>
+    <mergeCell ref="D51:D82"/>
+    <mergeCell ref="H51:H54"/>
+    <mergeCell ref="H59:H60"/>
+    <mergeCell ref="H57:H58"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="H70:H73"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="F80:F82"/>
+    <mergeCell ref="G80:G82"/>
+    <mergeCell ref="G29:G33"/>
+    <mergeCell ref="G51:G67"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="F51:F67"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="I70:I73"/>
+    <mergeCell ref="H48:H50"/>
+    <mergeCell ref="D29:D50"/>
+    <mergeCell ref="E29:E50"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="G5:G12"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="J3:N3"/>
+    <mergeCell ref="J5:J12"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="L5:L8"/>
+    <mergeCell ref="P5:P8"/>
+    <mergeCell ref="H5:H12"/>
+    <mergeCell ref="I5:I12"/>
+    <mergeCell ref="M5:M8"/>
+    <mergeCell ref="N5:N8"/>
+    <mergeCell ref="D5:D12"/>
+    <mergeCell ref="E5:E12"/>
+    <mergeCell ref="F5:F12"/>
+    <mergeCell ref="K5:K12"/>
+    <mergeCell ref="O5:O8"/>
+    <mergeCell ref="B5:B82"/>
+    <mergeCell ref="C5:C82"/>
+    <mergeCell ref="I74:I79"/>
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="F29:F33"/>
+    <mergeCell ref="D13:D28"/>
+    <mergeCell ref="L51:L54"/>
+    <mergeCell ref="J51:J54"/>
+    <mergeCell ref="K51:K54"/>
+    <mergeCell ref="M51:M54"/>
+    <mergeCell ref="N51:N54"/>
+    <mergeCell ref="I51:I54"/>
+    <mergeCell ref="I41:I43"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="L21:L23"/>
+    <mergeCell ref="J21:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="F16:F28"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="I21:I23"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="G34:G36"/>
+    <mergeCell ref="G16:G28"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I48:I50"/>
     <mergeCell ref="L62:L63"/>
     <mergeCell ref="M62:M63"/>
     <mergeCell ref="N62:N63"/>
@@ -4799,87 +4941,20 @@
     <mergeCell ref="N59:N60"/>
     <mergeCell ref="J62:J63"/>
     <mergeCell ref="K62:K63"/>
-    <mergeCell ref="L51:L54"/>
-    <mergeCell ref="J51:J54"/>
-    <mergeCell ref="K51:K54"/>
-    <mergeCell ref="M51:M54"/>
-    <mergeCell ref="N51:N54"/>
-    <mergeCell ref="I51:I54"/>
-    <mergeCell ref="I41:I43"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="L21:L23"/>
-    <mergeCell ref="J21:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="F16:F28"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="G34:G36"/>
-    <mergeCell ref="G16:G28"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="I48:I50"/>
-    <mergeCell ref="B2:S2"/>
-    <mergeCell ref="G5:G12"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="J3:N3"/>
-    <mergeCell ref="J5:J12"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="L5:L8"/>
-    <mergeCell ref="P5:P8"/>
-    <mergeCell ref="H5:H12"/>
-    <mergeCell ref="I5:I12"/>
-    <mergeCell ref="M5:M8"/>
-    <mergeCell ref="N5:N8"/>
-    <mergeCell ref="D5:D12"/>
-    <mergeCell ref="E5:E12"/>
-    <mergeCell ref="F5:F12"/>
-    <mergeCell ref="K5:K12"/>
-    <mergeCell ref="O5:O8"/>
-    <mergeCell ref="B5:B82"/>
-    <mergeCell ref="C5:C82"/>
-    <mergeCell ref="I74:I79"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="F29:F33"/>
-    <mergeCell ref="D13:D28"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="E51:E82"/>
-    <mergeCell ref="D51:D82"/>
-    <mergeCell ref="H51:H54"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="H70:H73"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="F80:F82"/>
-    <mergeCell ref="G80:G82"/>
-    <mergeCell ref="G29:G33"/>
-    <mergeCell ref="G51:G67"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="F51:F67"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="H62:H63"/>
-    <mergeCell ref="I70:I73"/>
-    <mergeCell ref="H48:H50"/>
-    <mergeCell ref="D29:D50"/>
-    <mergeCell ref="E29:E50"/>
-    <mergeCell ref="E13:E28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="F37:F50"/>
-    <mergeCell ref="G37:G50"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="F70:F79"/>
-    <mergeCell ref="G70:G79"/>
-    <mergeCell ref="H74:H79"/>
+    <mergeCell ref="N78:N79"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="J76:J77"/>
+    <mergeCell ref="K76:K77"/>
+    <mergeCell ref="N70:N73"/>
+    <mergeCell ref="L74:L75"/>
+    <mergeCell ref="L76:L77"/>
+    <mergeCell ref="N74:N75"/>
+    <mergeCell ref="N76:N77"/>
+    <mergeCell ref="J70:J73"/>
+    <mergeCell ref="L70:L73"/>
+    <mergeCell ref="K70:K73"/>
+    <mergeCell ref="M70:M73"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4890,8 +4965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A51" sqref="A1:A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A2:A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5104,7 +5179,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="28.5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A42" s="23" t="s">
         <v>403</v>
       </c>
@@ -5156,5 +5231,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>